<commit_message>
update and add TH06
</commit_message>
<xml_diff>
--- a/Day6/lophoc.xlsx
+++ b/Day6/lophoc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="11835"/>
+    <workbookView windowWidth="27945" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -100,14 +100,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,7 +253,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,12 +280,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -305,7 +292,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.6"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,12 +431,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -620,67 +601,70 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -695,46 +679,49 @@
     <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -743,10 +730,10 @@
     <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -755,17 +742,11 @@
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -783,7 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -792,15 +773,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -860,6 +842,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="5-Point Star 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9410700" y="2082800"/>
+          <a:ext cx="3724275" cy="4086225"/>
+        </a:xfrm>
+        <a:prstGeom prst="star5">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:srgbClr val="FFFFFF"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1122,8 +1170,8 @@
   <sheetPr/>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="2"/>
@@ -1135,10 +1183,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1231,13 +1279,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1"/>
@@ -1375,7 +1423,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:23">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1384,8 +1432,17 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1396,8 +1453,17 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1408,8 +1474,17 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1418,8 +1493,17 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1434,8 +1518,17 @@
         <v>17</v>
       </c>
       <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15"/>
+      <c r="W15" s="15"/>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
@@ -1456,8 +1549,17 @@
       <c r="H16" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1478,8 +1580,17 @@
       <c r="H17" s="10">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="10" t="s">
         <v>13</v>
       </c>
@@ -1500,8 +1611,17 @@
       <c r="H18" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="1"/>
@@ -1510,8 +1630,17 @@
       <c r="F19" s="1"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="11" t="s">
         <v>8</v>
       </c>
@@ -1526,6 +1655,158 @@
         <v>19</v>
       </c>
       <c r="H20" s="11"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+    </row>
+    <row r="21" spans="15:23">
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+    </row>
+    <row r="22" spans="15:23">
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+    </row>
+    <row r="23" spans="15:23">
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="15"/>
+    </row>
+    <row r="24" spans="15:23">
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+      <c r="W24" s="15"/>
+    </row>
+    <row r="25" spans="15:23">
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+      <c r="W25" s="15"/>
+    </row>
+    <row r="26" spans="15:23">
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+      <c r="V26" s="15"/>
+      <c r="W26" s="15"/>
+    </row>
+    <row r="27" spans="15:23">
+      <c r="O27" s="15"/>
+      <c r="P27" s="15"/>
+      <c r="Q27" s="15"/>
+      <c r="R27" s="15"/>
+      <c r="S27" s="15"/>
+      <c r="T27" s="15"/>
+      <c r="U27" s="15"/>
+      <c r="V27" s="15"/>
+      <c r="W27" s="15"/>
+    </row>
+    <row r="28" spans="15:23">
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
+      <c r="V28" s="15"/>
+      <c r="W28" s="15"/>
+    </row>
+    <row r="29" spans="15:23">
+      <c r="O29" s="15"/>
+      <c r="P29" s="15"/>
+      <c r="Q29" s="15"/>
+      <c r="R29" s="15"/>
+      <c r="S29" s="15"/>
+      <c r="T29" s="15"/>
+      <c r="U29" s="15"/>
+      <c r="V29" s="15"/>
+      <c r="W29" s="15"/>
+    </row>
+    <row r="30" spans="15:23">
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+    </row>
+    <row r="31" spans="15:23">
+      <c r="O31" s="15"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
+      <c r="S31" s="15"/>
+      <c r="T31" s="15"/>
+      <c r="U31" s="15"/>
+      <c r="V31" s="15"/>
+      <c r="W31" s="15"/>
+    </row>
+    <row r="32" spans="15:23">
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15"/>
+      <c r="U32" s="15"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="15"/>
+    </row>
+    <row r="33" spans="15:23">
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+      <c r="S33" s="15"/>
+      <c r="T33" s="15"/>
+      <c r="U33" s="15"/>
+      <c r="V33" s="15"/>
+      <c r="W33" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1542,5 +1823,6 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>